<commit_message>
update matlab logic and fix li's style string output
</commit_message>
<xml_diff>
--- a/DOC/慢检测逻辑判断.xlsx
+++ b/DOC/慢检测逻辑判断.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>bigmotion_time_vote</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -73,10 +73,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>当次大动作</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>大0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -93,19 +89,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>E连续出现三次</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>上一次是微1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>当次是F</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当次大动作B列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上一次是微1，c/d/e列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>后面一个周期还是F列的话连续输出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E连续出现三次，第三次出现时输出微1，并清掉等再连续出现时再输出微1，不连续出现就输出微0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -544,16 +548,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>
   <cols>
     <col min="1" max="1" width="28.1328125" customWidth="1"/>
-    <col min="2" max="2" width="22.265625" customWidth="1"/>
+    <col min="2" max="2" width="47.06640625" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="27.265625" customWidth="1"/>
     <col min="5" max="5" width="24.1328125" customWidth="1"/>
@@ -588,7 +592,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
@@ -627,10 +631,10 @@
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F4" s="11"/>
     </row>
@@ -660,28 +664,25 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
         <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="B10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="B11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -689,20 +690,33 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
         <v>12</v>
       </c>
-      <c r="B15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
       <c r="B16" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add output origin print
</commit_message>
<xml_diff>
--- a/DOC/慢检测逻辑判断.xlsx
+++ b/DOC/慢检测逻辑判断.xlsx
@@ -540,7 +540,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -551,7 +551,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>

</xml_diff>